<commit_message>
fix for env variables
</commit_message>
<xml_diff>
--- a/data/stocks.xlsx
+++ b/data/stocks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node_js\Puppeteer projects\web-scraping-basics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node_js\Puppeteer projects\stock-scraper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4514E70F-D634-4545-95D6-08F82F240E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC1AD1-9E62-46D3-881E-A05A1E4A815E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>URL</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>https://www.moneycontrol.com/india/stockpricequote/auto-lcvshcvs/eichermotors/EM</t>
-  </si>
-  <si>
-    <t>https://www.moneycontrol.com/india/stockpricequote/refineries/bharatpetroleumcorporation/BPC</t>
-  </si>
-  <si>
-    <t>https://www.moneycontrol.com/india/stockpricequote/pharmaceuticals/cadilahealthcare/CHC</t>
   </si>
   <si>
     <t>ID</t>
@@ -393,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -409,7 +403,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -437,29 +431,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>